<commit_message>
First attempt at replacing folders
First attempt at replacing folders
</commit_message>
<xml_diff>
--- a/01-Excel/2/Activities/02-Ins_NamedRanges/Solved/ShoppingTrip.xlsx
+++ b/01-Excel/2/Activities/02-Ins_NamedRanges/Solved/ShoppingTrip.xlsx
@@ -1,34 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\OneDrive\Documents\WorkAndSchool\TeachingAssistant\DataViz\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\2\Activities\02-Ins_NamedRanges\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\Desktop\GA Tech\GitHub\GT-ATL-DATA-PT-09-2020-U-C-2\01-Excel\2\Activities\02-Ins_NamedRanges\Solved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="DC6A508CB724DE4F1551BDFB3918CC2CF653C664" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{92A167DC-55F9-44DC-860D-3D15655D96C2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="443" windowWidth="25598" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="25605" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="Shopping Trip" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="ItemTable">'Shopping Trip'!$A$1:$D$6</definedName>
+    <definedName name="NewProducts">'Shopping Trip'!$A$7:$A$8</definedName>
     <definedName name="PaidTotal">'Shopping Trip'!$G$5</definedName>
     <definedName name="Prices">'Shopping Trip'!$B$2:$B$6</definedName>
     <definedName name="Products">'Shopping Trip'!$A$2:$A$6</definedName>
     <definedName name="Tax">'Shopping Trip'!$C$2:$C$6</definedName>
     <definedName name="TaxPrice">'Shopping Trip'!$D$2:$D$6</definedName>
+    <definedName name="TaxPrice2">'Shopping Trip'!$D$2:$D$19</definedName>
     <definedName name="TaxRate">'Shopping Trip'!$G$2</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Product</t>
   </si>
@@ -73,12 +71,18 @@
   </si>
   <si>
     <t>Gallon of Ice Cream</t>
+  </si>
+  <si>
+    <t>Sunscreen</t>
+  </si>
+  <si>
+    <t>Mentos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -180,7 +184,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{0E42069A-E08B-4EFF-B4B9-15BAA96C2BC3}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -492,22 +496,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.796875" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -543,7 +547,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -555,11 +559,11 @@
         <v>0.4</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D6" si="0">B3+C3</f>
+        <f t="shared" ref="D3:D8" si="0">B3+C3</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -578,7 +582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -598,7 +602,7 @@
         <v>72.599999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -612,6 +616,42 @@
       <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>36.299999999999997</v>
+      </c>
+      <c r="G6">
+        <f>SUM(TaxPrice2)</f>
+        <v>83.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <f>B7*TaxRate</f>
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <f>B8*TaxRate</f>
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>